<commit_message>
Added Database Class & Folder Restructure
</commit_message>
<xml_diff>
--- a/App/data/student_list.xlsx
+++ b/App/data/student_list.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADCBE3C-185C-42AB-B0DA-AF0BE6F2C0F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EF284-2E40-4758-9864-65527B3E5B15}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +36,6 @@
     <t xml:space="preserve">CHERN </t>
   </si>
   <si>
-    <t xml:space="preserve">KOH </t>
-  </si>
-  <si>
     <t xml:space="preserve">BRANDON </t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>KOH</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,7 +490,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -501,123 +501,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>